<commit_message>
Function 'create_ontology()' extended and new function for ontology visualisation implemented.
</commit_message>
<xml_diff>
--- a/ontology/ontology_use_case/quality_use_case_template.xlsx
+++ b/ontology/ontology_use_case/quality_use_case_template.xlsx
@@ -5,22 +5,25 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\A200093159\projects\product-knowledge\ontology\ontology_mapping\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\A200093159\projects\product-knowledge\ontology\ontology_use_case\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1088DE3-836A-4DB5-A1C9-37CDBD57781B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D60576F0-A945-403C-99CC-E50EC5D23A39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$I$1:$I$558</definedName>
+  </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2222" uniqueCount="649">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2236" uniqueCount="653">
   <si>
     <t>ontology</t>
   </si>
@@ -31,7 +34,7 @@
     <t>description</t>
   </si>
   <si>
-    <t>classattribute</t>
+    <t>class_attribute</t>
   </si>
   <si>
     <t>data_type</t>
@@ -49,10 +52,10 @@
     <t>relation_selection</t>
   </si>
   <si>
-    <t>consumer roles</t>
-  </si>
-  <si>
-    <t>provider roles</t>
+    <t>consumer_roles</t>
+  </si>
+  <si>
+    <t>provider_roles</t>
   </si>
   <si>
     <t># use case id</t>
@@ -1967,6 +1970,18 @@
   </si>
   <si>
     <t>bar</t>
+  </si>
+  <si>
+    <t>id_1</t>
+  </si>
+  <si>
+    <t>foo, bar</t>
+  </si>
+  <si>
+    <t>Diagnostic error codes are linked to data from internal quality tools to provide new insights.</t>
+  </si>
+  <si>
+    <t>Quality</t>
   </si>
 </sst>
 </file>
@@ -2394,8 +2409,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K558"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A202" workbookViewId="0">
-      <selection activeCell="F217" sqref="F217"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
@@ -2442,21 +2457,33 @@
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="B2" s="1" t="s">
+        <v>649</v>
+      </c>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="B3" s="1" t="s">
+        <v>652</v>
+      </c>
     </row>
     <row r="4" spans="1:11">
       <c r="A4" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="B4" s="1" t="s">
+        <v>651</v>
+      </c>
     </row>
     <row r="5" spans="1:11">
       <c r="A5" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="B5" s="1" t="s">
+        <v>650</v>
+      </c>
     </row>
     <row r="6" spans="1:11">
       <c r="A6" s="1" t="s">
@@ -2481,12 +2508,6 @@
       <c r="H9" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="I9" s="1" t="s">
-        <v>646</v>
-      </c>
-      <c r="J9" s="1" t="s">
-        <v>647</v>
-      </c>
     </row>
     <row r="10" spans="1:11">
       <c r="A10" s="1" t="s">
@@ -2571,12 +2592,6 @@
       <c r="E15" s="1" t="s">
         <v>483</v>
       </c>
-      <c r="F15" s="1" t="s">
-        <v>646</v>
-      </c>
-      <c r="J15" s="1" t="s">
-        <v>648</v>
-      </c>
     </row>
     <row r="16" spans="1:11">
       <c r="A16" s="1" t="s">
@@ -3488,7 +3503,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="81" spans="1:8">
+    <row r="81" spans="1:11">
       <c r="A81" s="1" t="s">
         <v>19</v>
       </c>
@@ -3502,7 +3517,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="82" spans="1:8">
+    <row r="82" spans="1:11">
       <c r="A82" s="1" t="s">
         <v>19</v>
       </c>
@@ -3516,7 +3531,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="83" spans="1:8">
+    <row r="83" spans="1:11">
       <c r="A83" s="1" t="s">
         <v>27</v>
       </c>
@@ -3530,7 +3545,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="84" spans="1:8">
+    <row r="84" spans="1:11">
       <c r="A84" s="1" t="s">
         <v>27</v>
       </c>
@@ -3544,7 +3559,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="85" spans="1:8">
+    <row r="85" spans="1:11">
       <c r="A85" s="1" t="s">
         <v>19</v>
       </c>
@@ -3558,7 +3573,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="86" spans="1:8">
+    <row r="86" spans="1:11">
       <c r="A86" s="1" t="s">
         <v>19</v>
       </c>
@@ -3572,7 +3587,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="87" spans="1:8">
+    <row r="87" spans="1:11">
       <c r="A87" s="1" t="s">
         <v>19</v>
       </c>
@@ -3586,7 +3601,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="88" spans="1:8">
+    <row r="88" spans="1:11">
       <c r="A88" s="1" t="s">
         <v>19</v>
       </c>
@@ -3600,7 +3615,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="89" spans="1:8">
+    <row r="89" spans="1:11">
       <c r="A89" s="1" t="s">
         <v>19</v>
       </c>
@@ -3614,7 +3629,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="90" spans="1:8">
+    <row r="90" spans="1:11">
       <c r="A90" s="1" t="s">
         <v>18</v>
       </c>
@@ -3628,7 +3643,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="91" spans="1:8">
+    <row r="91" spans="1:11">
       <c r="A91" s="1" t="s">
         <v>18</v>
       </c>
@@ -3642,7 +3657,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="92" spans="1:8">
+    <row r="92" spans="1:11">
       <c r="A92" s="1" t="s">
         <v>18</v>
       </c>
@@ -3656,7 +3671,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="93" spans="1:8">
+    <row r="93" spans="1:11">
       <c r="A93" s="1" t="s">
         <v>18</v>
       </c>
@@ -3669,8 +3684,17 @@
       <c r="H93" s="1" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="94" spans="1:8">
+      <c r="I93" s="1" t="s">
+        <v>646</v>
+      </c>
+      <c r="J93" s="1" t="s">
+        <v>647</v>
+      </c>
+      <c r="K93" s="1" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="94" spans="1:11">
       <c r="A94" s="1" t="s">
         <v>18</v>
       </c>
@@ -3684,7 +3708,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="95" spans="1:8">
+    <row r="95" spans="1:11">
       <c r="A95" s="1" t="s">
         <v>23</v>
       </c>
@@ -3698,7 +3722,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="96" spans="1:8">
+    <row r="96" spans="1:11">
       <c r="A96" s="1" t="s">
         <v>19</v>
       </c>
@@ -4160,7 +4184,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="129" spans="1:8">
+    <row r="129" spans="1:11">
       <c r="A129" s="1" t="s">
         <v>22</v>
       </c>
@@ -4174,7 +4198,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="130" spans="1:8">
+    <row r="130" spans="1:11">
       <c r="A130" s="1" t="s">
         <v>29</v>
       </c>
@@ -4188,7 +4212,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="131" spans="1:8">
+    <row r="131" spans="1:11">
       <c r="A131" s="1" t="s">
         <v>29</v>
       </c>
@@ -4202,7 +4226,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="132" spans="1:8">
+    <row r="132" spans="1:11">
       <c r="A132" s="1" t="s">
         <v>29</v>
       </c>
@@ -4216,7 +4240,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="133" spans="1:8">
+    <row r="133" spans="1:11">
       <c r="A133" s="1" t="s">
         <v>29</v>
       </c>
@@ -4230,7 +4254,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="134" spans="1:8">
+    <row r="134" spans="1:11">
       <c r="A134" s="1" t="s">
         <v>29</v>
       </c>
@@ -4244,7 +4268,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="135" spans="1:8">
+    <row r="135" spans="1:11">
       <c r="A135" s="1" t="s">
         <v>29</v>
       </c>
@@ -4258,7 +4282,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="136" spans="1:8">
+    <row r="136" spans="1:11">
       <c r="A136" s="1" t="s">
         <v>29</v>
       </c>
@@ -4271,8 +4295,17 @@
       <c r="H136" s="1" t="s">
         <v>608</v>
       </c>
-    </row>
-    <row r="137" spans="1:8">
+      <c r="I136" s="1" t="s">
+        <v>646</v>
+      </c>
+      <c r="J136" s="1" t="s">
+        <v>647</v>
+      </c>
+      <c r="K136" s="1" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="137" spans="1:11">
       <c r="A137" s="1" t="s">
         <v>29</v>
       </c>
@@ -4285,8 +4318,17 @@
       <c r="H137" s="1" t="s">
         <v>609</v>
       </c>
-    </row>
-    <row r="138" spans="1:8">
+      <c r="I137" s="1" t="s">
+        <v>646</v>
+      </c>
+      <c r="J137" s="1" t="s">
+        <v>647</v>
+      </c>
+      <c r="K137" s="1" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="138" spans="1:11">
       <c r="A138" s="1" t="s">
         <v>29</v>
       </c>
@@ -4299,8 +4341,17 @@
       <c r="H138" s="1" t="s">
         <v>610</v>
       </c>
-    </row>
-    <row r="139" spans="1:8">
+      <c r="I138" s="1" t="s">
+        <v>646</v>
+      </c>
+      <c r="J138" s="1" t="s">
+        <v>647</v>
+      </c>
+      <c r="K138" s="1" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="139" spans="1:11">
       <c r="A139" s="1" t="s">
         <v>29</v>
       </c>
@@ -4314,7 +4365,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="140" spans="1:8">
+    <row r="140" spans="1:11">
       <c r="A140" s="1" t="s">
         <v>29</v>
       </c>
@@ -4328,7 +4379,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="141" spans="1:8">
+    <row r="141" spans="1:11">
       <c r="A141" s="1" t="s">
         <v>29</v>
       </c>
@@ -4342,7 +4393,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="142" spans="1:8">
+    <row r="142" spans="1:11">
       <c r="A142" s="1" t="s">
         <v>29</v>
       </c>
@@ -4356,7 +4407,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="143" spans="1:8">
+    <row r="143" spans="1:11">
       <c r="A143" s="1" t="s">
         <v>29</v>
       </c>
@@ -4370,7 +4421,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="144" spans="1:8">
+    <row r="144" spans="1:11">
       <c r="A144" s="1" t="s">
         <v>29</v>
       </c>
@@ -5405,9 +5456,6 @@
       <c r="E217" s="1" t="s">
         <v>483</v>
       </c>
-      <c r="F217" s="1" t="s">
-        <v>646</v>
-      </c>
     </row>
     <row r="218" spans="1:8">
       <c r="A218" s="1" t="s">
@@ -5507,7 +5555,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="225" spans="1:8">
+    <row r="225" spans="1:11">
       <c r="A225" s="1" t="s">
         <v>20</v>
       </c>
@@ -5521,7 +5569,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="226" spans="1:8">
+    <row r="226" spans="1:11">
       <c r="A226" s="1" t="s">
         <v>20</v>
       </c>
@@ -5535,7 +5583,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="227" spans="1:8">
+    <row r="227" spans="1:11">
       <c r="A227" s="1" t="s">
         <v>20</v>
       </c>
@@ -5548,8 +5596,17 @@
       <c r="H227" s="1" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="228" spans="1:8">
+      <c r="I227" s="1" t="s">
+        <v>646</v>
+      </c>
+      <c r="J227" s="1" t="s">
+        <v>647</v>
+      </c>
+      <c r="K227" s="1" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="228" spans="1:11">
       <c r="A228" s="1" t="s">
         <v>20</v>
       </c>
@@ -5563,7 +5620,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="229" spans="1:8">
+    <row r="229" spans="1:11">
       <c r="A229" s="1" t="s">
         <v>20</v>
       </c>
@@ -5577,7 +5634,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="230" spans="1:8">
+    <row r="230" spans="1:11">
       <c r="A230" s="1" t="s">
         <v>23</v>
       </c>
@@ -5591,7 +5648,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="231" spans="1:8">
+    <row r="231" spans="1:11">
       <c r="A231" s="1" t="s">
         <v>23</v>
       </c>
@@ -5605,7 +5662,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="232" spans="1:8">
+    <row r="232" spans="1:11">
       <c r="A232" s="1" t="s">
         <v>26</v>
       </c>
@@ -5619,7 +5676,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="233" spans="1:8">
+    <row r="233" spans="1:11">
       <c r="A233" s="1" t="s">
         <v>17</v>
       </c>
@@ -5633,7 +5690,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="234" spans="1:8">
+    <row r="234" spans="1:11">
       <c r="A234" s="1" t="s">
         <v>26</v>
       </c>
@@ -5647,7 +5704,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="235" spans="1:8">
+    <row r="235" spans="1:11">
       <c r="A235" s="1" t="s">
         <v>17</v>
       </c>
@@ -5661,7 +5718,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="236" spans="1:8">
+    <row r="236" spans="1:11">
       <c r="A236" s="1" t="s">
         <v>26</v>
       </c>
@@ -5675,7 +5732,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="237" spans="1:8">
+    <row r="237" spans="1:11">
       <c r="A237" s="1" t="s">
         <v>17</v>
       </c>
@@ -5689,7 +5746,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="238" spans="1:8">
+    <row r="238" spans="1:11">
       <c r="A238" s="1" t="s">
         <v>26</v>
       </c>
@@ -5703,7 +5760,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="239" spans="1:8">
+    <row r="239" spans="1:11">
       <c r="A239" s="1" t="s">
         <v>17</v>
       </c>
@@ -5717,7 +5774,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="240" spans="1:8">
+    <row r="240" spans="1:11">
       <c r="A240" s="1" t="s">
         <v>26</v>
       </c>
@@ -10184,6 +10241,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="I1:I558" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <conditionalFormatting sqref="A1:A999">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>"class"</formula>

</xml_diff>